<commit_message>
Enhance reminder notification logic to include all active branch users. Updated the process reminder job to select branchId and notify relevant users, improving notification reach and clarity in logs.
</commit_message>
<xml_diff>
--- a/backend/templates/IchkiFSSMahsulotlariShabloni.xlsx
+++ b/backend/templates/IchkiFSSMahsulotlariShabloni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Prodeklarant\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27934569-2D8A-439E-B7EF-AB24A0CA80BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95775FC-8732-48C7-B438-827422EACD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,7 +223,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -237,6 +237,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -554,14 +560,14 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B4:B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="73.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="34.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -582,7 +588,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">

</xml_diff>